<commit_message>
Edit to BGDP for low GDP trajectory
</commit_message>
<xml_diff>
--- a/InputData/io-model/BGDP/BAU GDP.xlsx
+++ b/InputData/io-model/BGDP/BAU GDP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\io-model\BGDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42EE14D2-F5CA-4E3D-BCAF-EA1C01DC6C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3458D31-06C8-4FD6-8F47-BE25D335AF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1941,7 +1941,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1973,21 +1973,19 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3079,97 +3077,97 @@
                   <c:v>2611189004073.0547</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2822460696941.9834</c:v>
+                  <c:v>2773562143573.5303</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3050826414080.3457</c:v>
+                  <c:v>2946032229863.4243</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3307045553504.4199</c:v>
+                  <c:v>3134238110220.0601</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3584782878002.6206</c:v>
+                  <c:v>3334467434530.1445</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3885845560489.2153</c:v>
+                  <c:v>3547488314843.2466</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4212192546620.0317</c:v>
+                  <c:v>3774117933685.1636</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4565947301201.4443</c:v>
+                  <c:v>4015225678902.1641</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4949411625087.6543</c:v>
+                  <c:v>4271736478773.2793</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5365080632469.623</c:v>
+                  <c:v>4544634350184.6699</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5815658986009.4492</c:v>
+                  <c:v>4834966173477.4395</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6304078495458.4658</c:v>
+                  <c:v>5143845708449.8252</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6833517194269.2217</c:v>
+                  <c:v>5472457866919.7891</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>7407420018328.4746</c:v>
+                  <c:v>5814665194269.3955</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>8013201693706.3408</c:v>
+                  <c:v>6178271654831.0908</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>8668524428902.0117</c:v>
+                  <c:v>6564615393248.8701</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>9377439710957.1523</c:v>
+                  <c:v>6975118231905.9385</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>10144330359091.404</c:v>
+                  <c:v>7411290903516.0254</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>10973937621176.111</c:v>
+                  <c:v>7798938618498.1699</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>11682553238615.908</c:v>
+                  <c:v>8206862254758.6963</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>12436926004548.205</c:v>
+                  <c:v>8636122344754.7773</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>13240010576740.395</c:v>
+                  <c:v>9087834892114.4004</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>14094952402875.982</c:v>
+                  <c:v>9563174273057.0449</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>15005100040354.359</c:v>
+                  <c:v>10012590818237.223</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>15846879329561.463</c:v>
+                  <c:v>10483127466984.971</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>16735882054122.701</c:v>
+                  <c:v>10975776747900.957</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>17674757427288.199</c:v>
+                  <c:v>11491577832966.172</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>18666303281966.77</c:v>
+                  <c:v>12031618729524.029</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>19713474408221.195</c:v>
+                  <c:v>12597038575273.561</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>20819391358493.188</c:v>
+                  <c:v>13189030041114.652</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>21987349746797.477</c:v>
+                  <c:v>13808841846913.787</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>23220830069596.449</c:v>
+                  <c:v>14457781395496.918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3578,97 +3576,97 @@
                   <c:v>2611189004073.0547</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2418415626504.3853</c:v>
+                  <c:v>2376517071209.0532</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2832458205320.9595</c:v>
+                  <c:v>2735164847172.0952</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3188691783773.1221</c:v>
+                  <c:v>3022068837200.2329</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3520636110077.0586</c:v>
+                  <c:v>3274799857452.9722</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3851078540861.2144</c:v>
+                  <c:v>3515748608786.3921</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4193349108471.8076</c:v>
+                  <c:v>3757234242576.4639</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4555734313000.4092</c:v>
+                  <c:v>4006244530023.7417</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4943876269640.627</c:v>
+                  <c:v>4266959026102.7061</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5362080515430.2412</c:v>
+                  <c:v>4542093021193.4092</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5814032947295.9238</c:v>
+                  <c:v>4833614333179.4482</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6303197195874.7578</c:v>
+                  <c:v>5143126607460.7139</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6833039537157.0117</c:v>
+                  <c:v>5472075346711.3682</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7407420018328.4746</c:v>
+                  <c:v>5814665194269.3955</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8013201693706.3408</c:v>
+                  <c:v>6178271654831.0908</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8668524428902.0117</c:v>
+                  <c:v>6564615393248.8701</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9377439710957.1523</c:v>
+                  <c:v>6975118231905.9385</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10144330359091.404</c:v>
+                  <c:v>7411290903516.0254</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10973937621176.111</c:v>
+                  <c:v>7798938618498.1699</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11682553238615.908</c:v>
+                  <c:v>8206862254758.6963</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12436926004548.205</c:v>
+                  <c:v>8636122344754.7773</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13240010576740.395</c:v>
+                  <c:v>9087834892114.4004</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14094952402875.982</c:v>
+                  <c:v>9563174273057.0449</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15005100040354.359</c:v>
+                  <c:v>10012590818237.223</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15846879329561.463</c:v>
+                  <c:v>10483127466984.971</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>16735882054122.701</c:v>
+                  <c:v>10975776747900.957</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17674757427288.199</c:v>
+                  <c:v>11491577832966.172</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18666303281966.77</c:v>
+                  <c:v>12031618729524.029</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>19713474408221.195</c:v>
+                  <c:v>12597038575273.561</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20819391358493.188</c:v>
+                  <c:v>13189030041114.652</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21987349746797.477</c:v>
+                  <c:v>13808841846913.787</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>23220830069596.449</c:v>
+                  <c:v>14457781395496.918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5448,7 +5446,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>563</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -5456,7 +5454,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>564</v>
       </c>
       <c r="D7" s="3"/>
@@ -45293,8 +45291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45308,16 +45306,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" t="s">
         <v>566</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" t="s">
         <v>580</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" t="s">
         <v>581</v>
       </c>
-      <c r="D1" s="28"/>
       <c r="G1"/>
       <c r="H1"/>
     </row>
@@ -45419,32 +45416,32 @@
         <v>5.5730246037310319E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25">
+    <row r="7" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="24">
         <v>3</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>578</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>5.5657638964670221E-2</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <v>6.2183602660396575E-2</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <v>6.388452863781495E-2</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="26">
         <v>6.388452863781495E-2</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="26">
         <v>6.2532656380636584E-2</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="26">
         <v>5.2305019466748925E-2</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="26">
         <v>4.6994494960355127E-2</v>
       </c>
     </row>
@@ -45463,309 +45460,309 @@
       <c r="H9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="28">
+      <c r="A10">
         <v>2020</v>
       </c>
       <c r="B10" s="21">
-        <f>G$5</f>
-        <v>8.0910149567640269E-2</v>
+        <f>G$7</f>
+        <v>6.2183602660396575E-2</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="28">
+      <c r="A11">
         <v>2021</v>
       </c>
       <c r="B11" s="21">
-        <f t="shared" ref="B11:B12" si="0">G$5</f>
-        <v>8.0910149567640269E-2</v>
+        <f>G$7</f>
+        <v>6.2183602660396575E-2</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="28">
+      <c r="A12">
         <v>2022</v>
       </c>
       <c r="B12" s="21">
-        <f>H$5</f>
-        <v>8.3983519429869077E-2</v>
+        <f>H$7</f>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="28">
+      <c r="A13">
         <v>2023</v>
       </c>
       <c r="B13" s="21">
-        <f>H$5</f>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" ref="B13:B16" si="0">H$7</f>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="28">
+      <c r="A14">
         <v>2024</v>
       </c>
       <c r="B14" s="21">
-        <f t="shared" ref="B14:B17" si="1">H$5</f>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="28">
+      <c r="A15">
         <v>2025</v>
       </c>
       <c r="B15" s="21">
-        <f t="shared" si="1"/>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="28">
+      <c r="A16">
         <v>2026</v>
       </c>
       <c r="B16" s="21">
-        <f t="shared" si="1"/>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="28">
+      <c r="A17">
         <v>2027</v>
       </c>
       <c r="B17" s="21">
-        <f t="shared" si="1"/>
-        <v>8.3983519429869077E-2</v>
+        <f>I$7</f>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="28">
+      <c r="A18">
         <v>2028</v>
       </c>
       <c r="B18" s="21">
-        <f>I$5</f>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" ref="B18:B21" si="1">I$7</f>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="28">
+      <c r="A19">
         <v>2029</v>
       </c>
       <c r="B19" s="21">
-        <f t="shared" ref="B19:B22" si="2">I$5</f>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="28">
+      <c r="A20">
         <v>2030</v>
       </c>
       <c r="B20" s="21">
-        <f t="shared" si="2"/>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="28">
+      <c r="A21">
         <v>2031</v>
       </c>
       <c r="B21" s="21">
-        <f t="shared" si="2"/>
-        <v>8.3983519429869077E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.388452863781495E-2</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="28">
+      <c r="A22">
         <v>2032</v>
       </c>
       <c r="B22" s="21">
-        <f t="shared" si="2"/>
-        <v>8.3983519429869077E-2</v>
+        <f>J$7</f>
+        <v>6.2532656380636584E-2</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="28">
+      <c r="A23">
         <v>2033</v>
       </c>
       <c r="B23" s="21">
-        <f>J$5</f>
-        <v>8.1780386947001335E-2</v>
+        <f t="shared" ref="B23:B26" si="2">J$7</f>
+        <v>6.2532656380636584E-2</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="28">
+      <c r="A24">
         <v>2034</v>
       </c>
       <c r="B24" s="21">
-        <f t="shared" ref="B24:B27" si="3">J$5</f>
-        <v>8.1780386947001335E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.2532656380636584E-2</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="28">
+      <c r="A25">
         <v>2035</v>
       </c>
       <c r="B25" s="21">
-        <f t="shared" si="3"/>
-        <v>8.1780386947001335E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.2532656380636584E-2</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="28">
+      <c r="A26">
         <v>2036</v>
       </c>
       <c r="B26" s="21">
-        <f t="shared" si="3"/>
-        <v>8.1780386947001335E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.2532656380636584E-2</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="28">
+      <c r="A27">
         <v>2037</v>
       </c>
       <c r="B27" s="21">
-        <f t="shared" si="3"/>
-        <v>8.1780386947001335E-2</v>
+        <f>K$7</f>
+        <v>5.2305019466748925E-2</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="28">
+      <c r="A28">
         <v>2038</v>
       </c>
       <c r="B28" s="21">
-        <f>K$5</f>
-        <v>6.4572593894866109E-2</v>
+        <f t="shared" ref="B28:B31" si="3">K$7</f>
+        <v>5.2305019466748925E-2</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="28">
+      <c r="A29">
         <v>2039</v>
       </c>
       <c r="B29" s="21">
-        <f t="shared" ref="B29:B32" si="4">K$5</f>
-        <v>6.4572593894866109E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.2305019466748925E-2</v>
       </c>
       <c r="G29"/>
       <c r="H29"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="28">
+      <c r="A30">
         <v>2040</v>
       </c>
       <c r="B30" s="21">
-        <f t="shared" si="4"/>
-        <v>6.4572593894866109E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.2305019466748925E-2</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="28">
+      <c r="A31">
         <v>2041</v>
       </c>
       <c r="B31" s="21">
-        <f t="shared" si="4"/>
-        <v>6.4572593894866109E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.2305019466748925E-2</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="28">
+      <c r="A32">
         <v>2042</v>
       </c>
       <c r="B32" s="21">
-        <f t="shared" si="4"/>
-        <v>6.4572593894866109E-2</v>
+        <f>L$7</f>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G32"/>
       <c r="H32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="28">
+      <c r="A33">
         <v>2043</v>
       </c>
       <c r="B33" s="21">
-        <f>L$5</f>
-        <v>5.6099545284152841E-2</v>
+        <f t="shared" ref="B33:B36" si="4">L$7</f>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G33"/>
       <c r="H33"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="28">
+      <c r="A34">
         <v>2044</v>
       </c>
       <c r="B34" s="21">
-        <f t="shared" ref="B34:B40" si="5">L$5</f>
-        <v>5.6099545284152841E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G34"/>
       <c r="H34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="28">
+      <c r="A35">
         <v>2045</v>
       </c>
       <c r="B35" s="21">
-        <f t="shared" si="5"/>
-        <v>5.6099545284152841E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G35"/>
       <c r="H35"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="28">
+      <c r="A36">
         <v>2046</v>
       </c>
       <c r="B36" s="21">
-        <f t="shared" si="5"/>
-        <v>5.6099545284152841E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G36"/>
       <c r="H36"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="28">
+      <c r="A37">
         <v>2047</v>
       </c>
       <c r="B37" s="21">
-        <f t="shared" si="5"/>
-        <v>5.6099545284152841E-2</v>
+        <f>B36</f>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="C37" t="s">
         <v>583</v>
@@ -45778,34 +45775,34 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="28">
+      <c r="A38">
         <v>2048</v>
       </c>
       <c r="B38" s="21">
-        <f t="shared" si="5"/>
-        <v>5.6099545284152841E-2</v>
+        <f>B36</f>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G38"/>
       <c r="H38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="28">
+      <c r="A39">
         <v>2049</v>
       </c>
       <c r="B39" s="21">
-        <f t="shared" si="5"/>
-        <v>5.6099545284152841E-2</v>
+        <f>B36</f>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G39"/>
       <c r="H39"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="28">
+      <c r="A40">
         <v>2050</v>
       </c>
       <c r="B40" s="21">
-        <f t="shared" si="5"/>
-        <v>5.6099545284152841E-2</v>
+        <f>B36</f>
+        <v>4.6994494960355127E-2</v>
       </c>
       <c r="G40"/>
       <c r="H40"/>
@@ -46000,12 +45997,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -46817,7 +46814,7 @@
       <c r="A64" s="15">
         <v>2019</v>
       </c>
-      <c r="B64" s="23">
+      <c r="B64" s="10">
         <f>INDEX('World Bank_Real'!$113:$113,MATCH(Calcs!A64,'World Bank_Real'!$5:$5,0))</f>
         <v>2695611314661.46</v>
       </c>
@@ -46836,7 +46833,7 @@
       </c>
       <c r="C65" s="17">
         <f>C64*(1+IESS_LowGrowth!B10)</f>
-        <v>2822460696941.9834</v>
+        <v>2773562143573.5303</v>
       </c>
       <c r="D65">
         <v>2020</v>
@@ -46849,7 +46846,7 @@
       </c>
       <c r="G65" s="18">
         <f>C65*(1+E65)</f>
-        <v>2418415626504.3853</v>
+        <v>2376517071209.0532</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -46858,7 +46855,7 @@
       </c>
       <c r="C66" s="17">
         <f>C65*(1+IESS_LowGrowth!B11)</f>
-        <v>3050826414080.3457</v>
+        <v>2946032229863.4243</v>
       </c>
       <c r="D66">
         <v>2021</v>
@@ -46872,7 +46869,7 @@
       </c>
       <c r="G66" s="18">
         <f t="shared" ref="G66:G74" si="1">C66*(1+E66)</f>
-        <v>2832458205320.9595</v>
+        <v>2735164847172.0952</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -46881,7 +46878,7 @@
       </c>
       <c r="C67" s="17">
         <f>C66*(1+IESS_LowGrowth!B12)</f>
-        <v>3307045553504.4199</v>
+        <v>3134238110220.0601</v>
       </c>
       <c r="D67">
         <v>2022</v>
@@ -46895,7 +46892,7 @@
       </c>
       <c r="G67" s="18">
         <f t="shared" si="1"/>
-        <v>3188691783773.1221</v>
+        <v>3022068837200.2329</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -46904,7 +46901,7 @@
       </c>
       <c r="C68" s="17">
         <f>C67*(1+IESS_LowGrowth!B13)</f>
-        <v>3584782878002.6206</v>
+        <v>3334467434530.1445</v>
       </c>
       <c r="D68">
         <v>2023</v>
@@ -46918,7 +46915,7 @@
       </c>
       <c r="G68" s="18">
         <f t="shared" si="1"/>
-        <v>3520636110077.0586</v>
+        <v>3274799857452.9722</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -46927,7 +46924,7 @@
       </c>
       <c r="C69" s="17">
         <f>C68*(1+IESS_LowGrowth!B14)</f>
-        <v>3885845560489.2153</v>
+        <v>3547488314843.2466</v>
       </c>
       <c r="D69">
         <v>2024</v>
@@ -46941,7 +46938,7 @@
       </c>
       <c r="G69" s="18">
         <f t="shared" si="1"/>
-        <v>3851078540861.2144</v>
+        <v>3515748608786.3921</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -46950,7 +46947,7 @@
       </c>
       <c r="C70" s="17">
         <f>C69*(1+IESS_LowGrowth!B15)</f>
-        <v>4212192546620.0317</v>
+        <v>3774117933685.1636</v>
       </c>
       <c r="D70">
         <v>2025</v>
@@ -46964,7 +46961,7 @@
       </c>
       <c r="G70" s="18">
         <f t="shared" si="1"/>
-        <v>4193349108471.8076</v>
+        <v>3757234242576.4639</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -46973,7 +46970,7 @@
       </c>
       <c r="C71" s="17">
         <f>C70*(1+IESS_LowGrowth!B16)</f>
-        <v>4565947301201.4443</v>
+        <v>4015225678902.1641</v>
       </c>
       <c r="D71">
         <v>2026</v>
@@ -46987,7 +46984,7 @@
       </c>
       <c r="G71" s="18">
         <f t="shared" si="1"/>
-        <v>4555734313000.4092</v>
+        <v>4006244530023.7417</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -46996,7 +46993,7 @@
       </c>
       <c r="C72" s="17">
         <f>C71*(1+IESS_LowGrowth!B17)</f>
-        <v>4949411625087.6543</v>
+        <v>4271736478773.2793</v>
       </c>
       <c r="D72">
         <v>2027</v>
@@ -47010,7 +47007,7 @@
       </c>
       <c r="G72" s="18">
         <f t="shared" si="1"/>
-        <v>4943876269640.627</v>
+        <v>4266959026102.7061</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -47019,7 +47016,7 @@
       </c>
       <c r="C73" s="17">
         <f>C72*(1+IESS_LowGrowth!B18)</f>
-        <v>5365080632469.623</v>
+        <v>4544634350184.6699</v>
       </c>
       <c r="D73">
         <v>2028</v>
@@ -47033,7 +47030,7 @@
       </c>
       <c r="G73" s="18">
         <f t="shared" si="1"/>
-        <v>5362080515430.2412</v>
+        <v>4542093021193.4092</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -47042,7 +47039,7 @@
       </c>
       <c r="C74" s="17">
         <f>C73*(1+IESS_LowGrowth!B19)</f>
-        <v>5815658986009.4492</v>
+        <v>4834966173477.4395</v>
       </c>
       <c r="D74">
         <v>2029</v>
@@ -47056,7 +47053,7 @@
       </c>
       <c r="G74" s="18">
         <f t="shared" si="1"/>
-        <v>5814032947295.9238</v>
+        <v>4833614333179.4482</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -47065,7 +47062,7 @@
       </c>
       <c r="C75" s="17">
         <f>C74*(1+IESS_LowGrowth!B20)</f>
-        <v>6304078495458.4658</v>
+        <v>5143845708449.8252</v>
       </c>
       <c r="D75">
         <v>2030</v>
@@ -47079,7 +47076,7 @@
       </c>
       <c r="G75" s="18">
         <f>C75*(1+E75)</f>
-        <v>6303197195874.7578</v>
+        <v>5143126607460.7139</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -47088,7 +47085,7 @@
       </c>
       <c r="C76" s="17">
         <f>C75*(1+IESS_LowGrowth!B21)</f>
-        <v>6833517194269.2217</v>
+        <v>5472457866919.7891</v>
       </c>
       <c r="D76">
         <v>2031</v>
@@ -47102,7 +47099,7 @@
       </c>
       <c r="G76" s="18">
         <f>C76*(1+E76)</f>
-        <v>6833039537157.0117</v>
+        <v>5472075346711.3682</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -47111,11 +47108,11 @@
       </c>
       <c r="C77" s="17">
         <f>C76*(1+IESS_LowGrowth!B22)</f>
-        <v>7407420018328.4746</v>
+        <v>5814665194269.3955</v>
       </c>
       <c r="G77" s="18">
         <f t="shared" si="0"/>
-        <v>7407420018328.4746</v>
+        <v>5814665194269.3955</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -47124,11 +47121,11 @@
       </c>
       <c r="C78" s="17">
         <f>C77*(1+IESS_LowGrowth!B23)</f>
-        <v>8013201693706.3408</v>
+        <v>6178271654831.0908</v>
       </c>
       <c r="G78" s="18">
         <f t="shared" si="0"/>
-        <v>8013201693706.3408</v>
+        <v>6178271654831.0908</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -47137,11 +47134,11 @@
       </c>
       <c r="C79" s="17">
         <f>C78*(1+IESS_LowGrowth!B24)</f>
-        <v>8668524428902.0117</v>
+        <v>6564615393248.8701</v>
       </c>
       <c r="G79" s="18">
         <f t="shared" si="0"/>
-        <v>8668524428902.0117</v>
+        <v>6564615393248.8701</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -47150,11 +47147,11 @@
       </c>
       <c r="C80" s="17">
         <f>C79*(1+IESS_LowGrowth!B25)</f>
-        <v>9377439710957.1523</v>
+        <v>6975118231905.9385</v>
       </c>
       <c r="G80" s="18">
         <f t="shared" si="0"/>
-        <v>9377439710957.1523</v>
+        <v>6975118231905.9385</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -47163,11 +47160,11 @@
       </c>
       <c r="C81" s="17">
         <f>C80*(1+IESS_LowGrowth!B26)</f>
-        <v>10144330359091.404</v>
+        <v>7411290903516.0254</v>
       </c>
       <c r="G81" s="18">
         <f t="shared" si="0"/>
-        <v>10144330359091.404</v>
+        <v>7411290903516.0254</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -47176,11 +47173,11 @@
       </c>
       <c r="C82" s="17">
         <f>C81*(1+IESS_LowGrowth!B27)</f>
-        <v>10973937621176.111</v>
+        <v>7798938618498.1699</v>
       </c>
       <c r="G82" s="18">
         <f t="shared" si="0"/>
-        <v>10973937621176.111</v>
+        <v>7798938618498.1699</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -47189,11 +47186,11 @@
       </c>
       <c r="C83" s="17">
         <f>C82*(1+IESS_LowGrowth!B28)</f>
-        <v>11682553238615.908</v>
+        <v>8206862254758.6963</v>
       </c>
       <c r="G83" s="18">
         <f t="shared" si="0"/>
-        <v>11682553238615.908</v>
+        <v>8206862254758.6963</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -47202,11 +47199,11 @@
       </c>
       <c r="C84" s="17">
         <f>C83*(1+IESS_LowGrowth!B29)</f>
-        <v>12436926004548.205</v>
+        <v>8636122344754.7773</v>
       </c>
       <c r="G84" s="18">
         <f t="shared" si="0"/>
-        <v>12436926004548.205</v>
+        <v>8636122344754.7773</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -47215,11 +47212,11 @@
       </c>
       <c r="C85" s="17">
         <f>C84*(1+IESS_LowGrowth!B30)</f>
-        <v>13240010576740.395</v>
+        <v>9087834892114.4004</v>
       </c>
       <c r="G85" s="18">
         <f t="shared" si="0"/>
-        <v>13240010576740.395</v>
+        <v>9087834892114.4004</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -47228,11 +47225,11 @@
       </c>
       <c r="C86" s="17">
         <f>C85*(1+IESS_LowGrowth!B31)</f>
-        <v>14094952402875.982</v>
+        <v>9563174273057.0449</v>
       </c>
       <c r="G86" s="18">
         <f t="shared" si="0"/>
-        <v>14094952402875.982</v>
+        <v>9563174273057.0449</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -47241,11 +47238,11 @@
       </c>
       <c r="C87" s="17">
         <f>C86*(1+IESS_LowGrowth!B32)</f>
-        <v>15005100040354.359</v>
+        <v>10012590818237.223</v>
       </c>
       <c r="G87" s="18">
         <f t="shared" si="0"/>
-        <v>15005100040354.359</v>
+        <v>10012590818237.223</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -47254,11 +47251,11 @@
       </c>
       <c r="C88" s="17">
         <f>C87*(1+IESS_LowGrowth!B33)</f>
-        <v>15846879329561.463</v>
+        <v>10483127466984.971</v>
       </c>
       <c r="G88" s="18">
         <f t="shared" si="0"/>
-        <v>15846879329561.463</v>
+        <v>10483127466984.971</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -47267,11 +47264,11 @@
       </c>
       <c r="C89" s="17">
         <f>C88*(1+IESS_LowGrowth!B34)</f>
-        <v>16735882054122.701</v>
+        <v>10975776747900.957</v>
       </c>
       <c r="G89" s="18">
         <f t="shared" si="0"/>
-        <v>16735882054122.701</v>
+        <v>10975776747900.957</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -47280,11 +47277,11 @@
       </c>
       <c r="C90" s="17">
         <f>C89*(1+IESS_LowGrowth!B35)</f>
-        <v>17674757427288.199</v>
+        <v>11491577832966.172</v>
       </c>
       <c r="G90" s="18">
         <f t="shared" si="0"/>
-        <v>17674757427288.199</v>
+        <v>11491577832966.172</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -47293,11 +47290,11 @@
       </c>
       <c r="C91" s="17">
         <f>C90*(1+IESS_LowGrowth!B36)</f>
-        <v>18666303281966.77</v>
+        <v>12031618729524.029</v>
       </c>
       <c r="G91" s="18">
         <f t="shared" si="0"/>
-        <v>18666303281966.77</v>
+        <v>12031618729524.029</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -47306,11 +47303,11 @@
       </c>
       <c r="C92" s="17">
         <f>C91*(1+IESS_LowGrowth!B37)</f>
-        <v>19713474408221.195</v>
+        <v>12597038575273.561</v>
       </c>
       <c r="G92" s="18">
         <f t="shared" si="0"/>
-        <v>19713474408221.195</v>
+        <v>12597038575273.561</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -47319,11 +47316,11 @@
       </c>
       <c r="C93" s="17">
         <f>C92*(1+IESS_LowGrowth!B38)</f>
-        <v>20819391358493.188</v>
+        <v>13189030041114.652</v>
       </c>
       <c r="G93" s="18">
         <f t="shared" si="0"/>
-        <v>20819391358493.188</v>
+        <v>13189030041114.652</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -47332,11 +47329,11 @@
       </c>
       <c r="C94" s="17">
         <f>C93*(1+IESS_LowGrowth!B39)</f>
-        <v>21987349746797.477</v>
+        <v>13808841846913.787</v>
       </c>
       <c r="G94" s="18">
         <f t="shared" si="0"/>
-        <v>21987349746797.477</v>
+        <v>13808841846913.787</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -47345,11 +47342,11 @@
       </c>
       <c r="C95" s="17">
         <f>C94*(1+IESS_LowGrowth!B40)</f>
-        <v>23220830069596.449</v>
+        <v>14457781395496.918</v>
       </c>
       <c r="G95" s="18">
         <f t="shared" si="0"/>
-        <v>23220830069596.449</v>
+        <v>14457781395496.918</v>
       </c>
     </row>
   </sheetData>
@@ -47370,8 +47367,8 @@
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47445,7 +47442,7 @@
       </c>
       <c r="B7" s="18">
         <f>Calcs!G65</f>
-        <v>2418415626504.3853</v>
+        <v>2376517071209.0532</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -47455,7 +47452,7 @@
       </c>
       <c r="B8" s="18">
         <f>Calcs!G66</f>
-        <v>2832458205320.9595</v>
+        <v>2735164847172.0952</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -47465,7 +47462,7 @@
       </c>
       <c r="B9" s="18">
         <f>Calcs!G67</f>
-        <v>3188691783773.1221</v>
+        <v>3022068837200.2329</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -47475,7 +47472,7 @@
       </c>
       <c r="B10" s="18">
         <f>Calcs!G68</f>
-        <v>3520636110077.0586</v>
+        <v>3274799857452.9722</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -47485,7 +47482,7 @@
       </c>
       <c r="B11" s="18">
         <f>Calcs!G69</f>
-        <v>3851078540861.2144</v>
+        <v>3515748608786.3921</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -47495,7 +47492,7 @@
       </c>
       <c r="B12" s="18">
         <f>Calcs!G70</f>
-        <v>4193349108471.8076</v>
+        <v>3757234242576.4639</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -47505,7 +47502,7 @@
       </c>
       <c r="B13" s="18">
         <f>Calcs!G71</f>
-        <v>4555734313000.4092</v>
+        <v>4006244530023.7417</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -47515,7 +47512,7 @@
       </c>
       <c r="B14" s="18">
         <f>Calcs!G72</f>
-        <v>4943876269640.627</v>
+        <v>4266959026102.7061</v>
       </c>
       <c r="C14" s="6"/>
     </row>
@@ -47525,7 +47522,7 @@
       </c>
       <c r="B15" s="18">
         <f>Calcs!G73</f>
-        <v>5362080515430.2412</v>
+        <v>4542093021193.4092</v>
       </c>
       <c r="C15" s="6"/>
     </row>
@@ -47535,7 +47532,7 @@
       </c>
       <c r="B16" s="18">
         <f>Calcs!G74</f>
-        <v>5814032947295.9238</v>
+        <v>4833614333179.4482</v>
       </c>
       <c r="C16" s="6"/>
     </row>
@@ -47545,7 +47542,7 @@
       </c>
       <c r="B17" s="18">
         <f>Calcs!G75</f>
-        <v>6303197195874.7578</v>
+        <v>5143126607460.7139</v>
       </c>
       <c r="C17" s="6"/>
     </row>
@@ -47555,7 +47552,7 @@
       </c>
       <c r="B18" s="18">
         <f>Calcs!G76</f>
-        <v>6833039537157.0117</v>
+        <v>5472075346711.3682</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -47565,7 +47562,7 @@
       </c>
       <c r="B19" s="18">
         <f>Calcs!G77</f>
-        <v>7407420018328.4746</v>
+        <v>5814665194269.3955</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -47575,7 +47572,7 @@
       </c>
       <c r="B20" s="18">
         <f>Calcs!G78</f>
-        <v>8013201693706.3408</v>
+        <v>6178271654831.0908</v>
       </c>
       <c r="C20" s="6"/>
     </row>
@@ -47585,7 +47582,7 @@
       </c>
       <c r="B21" s="18">
         <f>Calcs!G79</f>
-        <v>8668524428902.0117</v>
+        <v>6564615393248.8701</v>
       </c>
       <c r="C21" s="6"/>
     </row>
@@ -47595,7 +47592,7 @@
       </c>
       <c r="B22" s="18">
         <f>Calcs!G80</f>
-        <v>9377439710957.1523</v>
+        <v>6975118231905.9385</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -47605,7 +47602,7 @@
       </c>
       <c r="B23" s="18">
         <f>Calcs!G81</f>
-        <v>10144330359091.404</v>
+        <v>7411290903516.0254</v>
       </c>
       <c r="C23" s="6"/>
     </row>
@@ -47615,7 +47612,7 @@
       </c>
       <c r="B24" s="18">
         <f>Calcs!G82</f>
-        <v>10973937621176.111</v>
+        <v>7798938618498.1699</v>
       </c>
       <c r="C24" s="6"/>
     </row>
@@ -47625,7 +47622,7 @@
       </c>
       <c r="B25" s="18">
         <f>Calcs!G83</f>
-        <v>11682553238615.908</v>
+        <v>8206862254758.6963</v>
       </c>
       <c r="C25" s="6"/>
     </row>
@@ -47635,7 +47632,7 @@
       </c>
       <c r="B26" s="18">
         <f>Calcs!G84</f>
-        <v>12436926004548.205</v>
+        <v>8636122344754.7773</v>
       </c>
       <c r="C26" s="6"/>
     </row>
@@ -47645,7 +47642,7 @@
       </c>
       <c r="B27" s="18">
         <f>Calcs!G85</f>
-        <v>13240010576740.395</v>
+        <v>9087834892114.4004</v>
       </c>
       <c r="C27" s="6"/>
     </row>
@@ -47655,7 +47652,7 @@
       </c>
       <c r="B28" s="18">
         <f>Calcs!G86</f>
-        <v>14094952402875.982</v>
+        <v>9563174273057.0449</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -47665,7 +47662,7 @@
       </c>
       <c r="B29" s="18">
         <f>Calcs!G87</f>
-        <v>15005100040354.359</v>
+        <v>10012590818237.223</v>
       </c>
       <c r="C29" s="6"/>
     </row>
@@ -47675,7 +47672,7 @@
       </c>
       <c r="B30" s="18">
         <f>Calcs!G88</f>
-        <v>15846879329561.463</v>
+        <v>10483127466984.971</v>
       </c>
       <c r="C30" s="6"/>
     </row>
@@ -47685,7 +47682,7 @@
       </c>
       <c r="B31" s="18">
         <f>Calcs!G89</f>
-        <v>16735882054122.701</v>
+        <v>10975776747900.957</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -47695,7 +47692,7 @@
       </c>
       <c r="B32" s="18">
         <f>Calcs!G90</f>
-        <v>17674757427288.199</v>
+        <v>11491577832966.172</v>
       </c>
       <c r="C32" s="6"/>
     </row>
@@ -47705,7 +47702,7 @@
       </c>
       <c r="B33" s="18">
         <f>Calcs!G91</f>
-        <v>18666303281966.77</v>
+        <v>12031618729524.029</v>
       </c>
       <c r="C33" s="6"/>
     </row>
@@ -47715,7 +47712,7 @@
       </c>
       <c r="B34" s="18">
         <f>Calcs!G92</f>
-        <v>19713474408221.195</v>
+        <v>12597038575273.561</v>
       </c>
       <c r="C34" s="6"/>
     </row>
@@ -47725,7 +47722,7 @@
       </c>
       <c r="B35" s="18">
         <f>Calcs!G93</f>
-        <v>20819391358493.188</v>
+        <v>13189030041114.652</v>
       </c>
       <c r="C35" s="6"/>
     </row>
@@ -47735,7 +47732,7 @@
       </c>
       <c r="B36" s="18">
         <f>Calcs!G94</f>
-        <v>21987349746797.477</v>
+        <v>13808841846913.787</v>
       </c>
       <c r="C36" s="6"/>
     </row>
@@ -47745,7 +47742,7 @@
       </c>
       <c r="B37" s="18">
         <f>Calcs!G95</f>
-        <v>23220830069596.449</v>
+        <v>14457781395496.918</v>
       </c>
       <c r="C37" s="6"/>
     </row>

</xml_diff>